<commit_message>
[add] Question dialog for asking fill member data at first for demo
</commit_message>
<xml_diff>
--- a/sample_9_people.xlsx
+++ b/sample_9_people.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="member" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="431">
   <si>
     <t xml:space="preserve">id_name</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">id_contact_tel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sloss Huang</t>
   </si>
   <si>
     <t xml:space="preserve">0918523189</t>
@@ -158,9 +155,6 @@
     <t xml:space="preserve">Kelly Huang</t>
   </si>
   <si>
-    <t xml:space="preserve">Cacy Huang</t>
-  </si>
-  <si>
     <t xml:space="preserve">0918523190</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t xml:space="preserve">A210466111</t>
   </si>
   <si>
-    <t xml:space="preserve">Jimmy Huang</t>
-  </si>
-  <si>
     <t xml:space="preserve">0918523191</t>
   </si>
   <si>
@@ -244,9 +235,6 @@
     <t xml:space="preserve">男</t>
   </si>
   <si>
-    <t xml:space="preserve">Lucy Cheng</t>
-  </si>
-  <si>
     <t xml:space="preserve">0918523192</t>
   </si>
   <si>
@@ -257,9 +245,6 @@
   </si>
   <si>
     <t xml:space="preserve">A247610447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terry Huang</t>
   </si>
   <si>
     <t xml:space="preserve">0918523193</t>
@@ -1653,26 +1638,26 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,38 +1711,38 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>1951</v>
@@ -1769,45 +1754,45 @@
         <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>1961</v>
@@ -1819,45 +1804,45 @@
         <v>28</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>1971</v>
@@ -1869,45 +1854,45 @@
         <v>28</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L5" s="3" t="n">
         <v>1981</v>
@@ -1919,45 +1904,45 @@
         <v>28</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>43</v>
+      <c r="A6" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J6" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L6" s="3" t="n">
         <v>1991</v>
@@ -1969,45 +1954,45 @@
         <v>28</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J7" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L7" s="3" t="n">
         <v>2001</v>
@@ -2019,45 +2004,45 @@
         <v>28</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J8" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L8" s="3" t="n">
         <v>2011</v>
@@ -2069,45 +2054,45 @@
         <v>28</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J9" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L9" s="3" t="n">
         <v>1950</v>
@@ -2119,45 +2104,45 @@
         <v>28</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L10" s="3" t="n">
         <v>1973</v>
@@ -2169,10 +2154,10 @@
         <v>28</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2437,16 +2422,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -2488,1221 +2470,1221 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="R5" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="T5" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="V5" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="W5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="X5" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="Y5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="Z5" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="AA5" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="AB5" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="X5" s="11" t="s">
+      <c r="AC5" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="AD5" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="AE5" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="AA5" s="11" t="s">
+      <c r="AF5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AB5" s="11" t="s">
+      <c r="AG5" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="AH5" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AD5" s="11" t="s">
+      <c r="AI5" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="AE5" s="11" t="s">
+      <c r="AJ5" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AF5" s="11" t="s">
+      <c r="AK5" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AG5" s="11" t="s">
+      <c r="AL5" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AH5" s="11" t="s">
+      <c r="AM5" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="AI5" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ5" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK5" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL5" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM5" s="11" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="T6" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="U6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="V6" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="W6" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="X6" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="Y6" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="AC6" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="AD6" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA6" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB6" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC6" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD6" s="11" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="M7" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="M8" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="N8" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="I10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="L10" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="M10" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="N10" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="M11" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="N11" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="O11" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="P11" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="Q11" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="R11" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="S11" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q11" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="R11" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="S11" s="11" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="L12" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="M12" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="N12" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="O12" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="P12" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="Q12" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="R12" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="S12" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="T12" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="P12" s="11" t="s">
+      <c r="U12" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="Q12" s="11" t="s">
+      <c r="V12" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="R12" s="11" t="s">
+      <c r="W12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="X12" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="S12" s="11" t="s">
+      <c r="Y12" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="T12" s="11" t="s">
+      <c r="Z12" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="U12" s="11" t="s">
+      <c r="AA12" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="V12" s="11" t="s">
+      <c r="AB12" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="W12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="X12" s="11" t="s">
+      <c r="AC12" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="Y12" s="11" t="s">
+      <c r="AD12" s="11" t="s">
         <v>228</v>
-      </c>
-      <c r="Z12" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA12" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AB12" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="AC12" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="AD12" s="11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="L13" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="M13" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="N13" s="11" t="s">
         <v>242</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="L14" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="11" t="s">
+      <c r="M14" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="N14" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="O14" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="P14" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="Q14" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="R14" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="S14" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="T14" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="U14" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="V14" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="W14" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="X14" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="T14" s="11" t="s">
+      <c r="Y14" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="U14" s="11" t="s">
+      <c r="Z14" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="V14" s="11" t="s">
+      <c r="AA14" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="W14" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="X14" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="Y14" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="Z14" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="AA14" s="11" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="J16" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="L16" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="M16" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="N16" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="O16" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="P16" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="Q16" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="R16" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="O16" s="11" t="s">
+      <c r="T16" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="U16" s="11" t="s">
         <v>290</v>
-      </c>
-      <c r="Q16" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="U16" s="11" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="J17" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="L17" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="M17" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="N17" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="O17" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="P17" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="Q17" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="R17" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="S17" s="11" t="s">
         <v>309</v>
-      </c>
-      <c r="O17" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="P17" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="R17" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="S17" s="11" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="J18" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="K18" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="L18" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="M18" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="N18" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="O18" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="P18" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="Q18" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="R18" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="S18" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="T18" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="P18" s="11" t="s">
+      <c r="U18" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="V18" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="W18" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="S18" s="11" t="s">
+      <c r="X18" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="T18" s="11" t="s">
+      <c r="Y18" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="U18" s="11" t="s">
+      <c r="Z18" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="V18" s="11" t="s">
+      <c r="AA18" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="W18" s="11" t="s">
+      <c r="AB18" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="X18" s="11" t="s">
+      <c r="AC18" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="Y18" s="11" t="s">
+      <c r="AD18" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="Z18" s="11" t="s">
+      <c r="AE18" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="AA18" s="11" t="s">
+      <c r="AF18" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="AB18" s="11" t="s">
+      <c r="AG18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH18" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI18" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ18" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="AC18" s="11" t="s">
+      <c r="AK18" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="AD18" s="11" t="s">
+      <c r="AL18" s="11" t="s">
         <v>344</v>
-      </c>
-      <c r="AE18" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="AF18" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="AG18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH18" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI18" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ18" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="AK18" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="AL18" s="11" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="J19" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="L19" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="M19" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="N19" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="O19" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="P19" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="Q19" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="R19" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="S19" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="O19" s="11" t="s">
+      <c r="T19" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="P19" s="11" t="s">
+      <c r="U19" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="Q19" s="11" t="s">
+      <c r="V19" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="W19" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="S19" s="11" t="s">
+      <c r="X19" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="T19" s="11" t="s">
+      <c r="Y19" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="U19" s="11" t="s">
+      <c r="Z19" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="V19" s="11" t="s">
+      <c r="AA19" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="W19" s="11" t="s">
+      <c r="AB19" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="X19" s="11" t="s">
+      <c r="AC19" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="Y19" s="11" t="s">
+      <c r="AD19" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="Z19" s="11" t="s">
+      <c r="AE19" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="AA19" s="11" t="s">
+      <c r="AF19" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="AB19" s="11" t="s">
+      <c r="AG19" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="AC19" s="11" t="s">
+      <c r="AH19" s="11" t="s">
         <v>378</v>
-      </c>
-      <c r="AD19" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="AE19" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="AF19" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="AG19" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="AH19" s="11" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="L20" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="M20" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="N20" s="11" t="s">
         <v>392</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="N20" s="11" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="L21" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="M21" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="N21" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="O21" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="P21" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="Q21" s="11" t="s">
         <v>409</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="O21" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="P21" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q21" s="11" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>415</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>422</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -3732,16 +3714,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3757,13 +3739,13 @@
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>